<commit_message>
Made changes in click method
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/TestDataGradeFour.xlsx
+++ b/src/main/resources/testData/TestDataGradeFour.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="140">
   <si>
     <t>Password</t>
   </si>
@@ -344,6 +344,114 @@
   </si>
   <si>
     <t>27585107</t>
+  </si>
+  <si>
+    <t>rcg+27585128@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585128</t>
+  </si>
+  <si>
+    <t>27585128</t>
+  </si>
+  <si>
+    <t>rcg+27585144@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585144</t>
+  </si>
+  <si>
+    <t>27585144</t>
+  </si>
+  <si>
+    <t>rcg+27585146@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585146</t>
+  </si>
+  <si>
+    <t>27585146</t>
+  </si>
+  <si>
+    <t>rcg+27585149@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585149</t>
+  </si>
+  <si>
+    <t>27585149</t>
+  </si>
+  <si>
+    <t>rcg+27585154@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585154</t>
+  </si>
+  <si>
+    <t>27585154</t>
+  </si>
+  <si>
+    <t>rcg+27585160@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585160</t>
+  </si>
+  <si>
+    <t>27585160</t>
+  </si>
+  <si>
+    <t>rcg+27585167@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585167</t>
+  </si>
+  <si>
+    <t>27585167</t>
+  </si>
+  <si>
+    <t>rcg+27585169@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585169</t>
+  </si>
+  <si>
+    <t>27585169</t>
+  </si>
+  <si>
+    <t>rcg+27585174@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585174</t>
+  </si>
+  <si>
+    <t>27585174</t>
+  </si>
+  <si>
+    <t>rcg+27585182@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585182</t>
+  </si>
+  <si>
+    <t>27585182</t>
+  </si>
+  <si>
+    <t>rcg+27585191@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585191</t>
+  </si>
+  <si>
+    <t>27585191</t>
+  </si>
+  <si>
+    <t>rcg+27585195@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585195</t>
+  </si>
+  <si>
+    <t>27585195</t>
   </si>
 </sst>
 </file>
@@ -923,16 +1031,16 @@
     </row>
     <row r="2" spans="1:4" ht="16">
       <c r="A2" s="7" t="s">
-        <v>101</v>
+        <v>137</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16">

</xml_diff>